<commit_message>
tournament closure exception handeled
</commit_message>
<xml_diff>
--- a/tournament/matches/Chennai_SouthAfrica_vs_Mumbai_India.xlsx
+++ b/tournament/matches/Chennai_SouthAfrica_vs_Mumbai_India.xlsx
@@ -527,14 +527,14 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
         <v>3</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -551,14 +551,14 @@
         </is>
       </c>
       <c r="K2" t="n">
+        <v>39</v>
+      </c>
+      <c r="L2" t="n">
         <v>14</v>
       </c>
-      <c r="L2" t="n">
-        <v>7</v>
-      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -577,19 +577,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mohommad Shami</t>
+          <t xml:space="preserve"> Jasprit Bumrah</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -601,19 +601,19 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="L3" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Kagiso Rabada</t>
+          <t xml:space="preserve"> Anrich Nortje</t>
         </is>
       </c>
       <c r="O3" t="n">
@@ -627,19 +627,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Kuldeep Yadav</t>
+          <t xml:space="preserve"> Bhuvneshwar Kumar</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -651,14 +651,14 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -677,14 +677,14 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" t="n">
         <v>22</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -701,19 +701,19 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="L5" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Anrich Nortje</t>
+          <t xml:space="preserve"> Kagiso Rabada</t>
         </is>
       </c>
       <c r="O5" t="n">
@@ -727,10 +727,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -739,7 +739,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Bhuvneshwar Kumar</t>
+          <t xml:space="preserve"> Kuldeep Yadav</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -751,19 +751,19 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="L6" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tabraiz Shamsi</t>
+          <t xml:space="preserve"> Keshav Maharaj</t>
         </is>
       </c>
       <c r="O6" t="n">
@@ -777,19 +777,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mohommad Shami</t>
+          <t xml:space="preserve"> Bhuvneshwar Kumar</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -801,19 +801,19 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Anrich Nortje</t>
+          <t xml:space="preserve"> Kagiso Rabada</t>
         </is>
       </c>
       <c r="O7" t="n">
@@ -827,19 +827,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mohommad Shami</t>
+          <t xml:space="preserve"> Hardik Pandya</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -851,19 +851,19 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="L8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Keshav Maharaj</t>
+          <t xml:space="preserve"> Tabraiz Shamsi</t>
         </is>
       </c>
       <c r="O8" t="n">
@@ -877,19 +877,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Hardik Pandya</t>
+          <t xml:space="preserve"> Mohommad Shami</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -901,19 +901,19 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>NOT OUT</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Anrich Nortje</t>
         </is>
       </c>
       <c r="O9" t="n">
@@ -927,19 +927,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t>* NOT OUT</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Bhuvneshwar Kumar</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -951,10 +951,10 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -977,19 +977,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>NOT OUT</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mohommad Shami</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1001,19 +1001,19 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="L11" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>NOT OUT</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Kagiso Rabada</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="O11" t="n">
@@ -1027,14 +1027,14 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>NOT OUT</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1051,10 +1051,10 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dwaine Pretorius</t>
+          <t xml:space="preserve"> Anrich Nortje</t>
         </is>
       </c>
       <c r="O12" t="n">
@@ -1114,32 +1114,32 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>191</v>
+        <v>307</v>
       </c>
       <c r="B16" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>12.2</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="J16" t="n">
-        <v>141</v>
+        <v>233</v>
       </c>
       <c r="K16" t="n">
         <v>10</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>16.3</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>58</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20">
@@ -1197,201 +1197,201 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Bhuvneshwar Kumar</t>
+          <t>Kuldeep Yadav</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D21" t="n">
         <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>14</v>
+        <v>13.25</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Tabraiz Shamsi</t>
+          <t>Keshav Maharaj</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="M21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N21" t="n">
-        <v>13</v>
+        <v>16.33</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Hardik Pandya</t>
+          <t>Jasprit Bumrah</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
         <v>18</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Anrich Nortje</t>
+          <t>Kagiso Rabada</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="M22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N22" t="n">
-        <v>10.5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Kuldeep Yadav</t>
+          <t>Mohommad Shami</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>62</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Dwaine Pretorius</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
           <t>3.0</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>46</v>
-      </c>
-      <c r="D23" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" t="n">
-        <v>15.33</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Keshav Maharaj</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
       <c r="L23" t="n">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="M23" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>16.5</v>
+        <v>14.33</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Jasprit Bumrah</t>
+          <t>Bhuvneshwar Kumar</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" t="n">
+        <v>15</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Tabraiz Shamsi</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>55</v>
+      </c>
+      <c r="M24" t="n">
         <v>1</v>
       </c>
-      <c r="E24" t="n">
-        <v>15.67</v>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>Kagiso Rabada</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="L24" t="n">
-        <v>29</v>
-      </c>
-      <c r="M24" t="n">
-        <v>3</v>
-      </c>
       <c r="N24" t="n">
-        <v>14.5</v>
+        <v>13.75</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Mohommad Shami</t>
+          <t>Hardik Pandya</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>15.45</v>
+        <v>15</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Dwaine Pretorius</t>
+          <t>Anrich Nortje</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="M25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N25" t="n">
-        <v>22.86</v>
+        <v>13.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
main loop error fixed ------toss_nadun
</commit_message>
<xml_diff>
--- a/tournament/matches/Chennai_SouthAfrica_vs_Mumbai_India.xlsx
+++ b/tournament/matches/Chennai_SouthAfrica_vs_Mumbai_India.xlsx
@@ -527,19 +527,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Kuldeep Yadav</t>
+          <t xml:space="preserve"> Mohommad Shami</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -551,19 +551,19 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="L2" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Keshav Maharaj</t>
+          <t xml:space="preserve"> Kagiso Rabada</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -577,19 +577,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Jasprit Bumrah</t>
+          <t xml:space="preserve"> Bhuvneshwar Kumar</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -601,11 +601,11 @@
         </is>
       </c>
       <c r="K3" t="n">
+        <v>34</v>
+      </c>
+      <c r="L3" t="n">
         <v>10</v>
       </c>
-      <c r="L3" t="n">
-        <v>4</v>
-      </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>Caught</t>
@@ -613,7 +613,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Anrich Nortje</t>
+          <t xml:space="preserve"> Keshav Maharaj</t>
         </is>
       </c>
       <c r="O3" t="n">
@@ -627,19 +627,19 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>33</v>
+      </c>
+      <c r="C4" t="n">
         <v>14</v>
       </c>
-      <c r="C4" t="n">
-        <v>7</v>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Bhuvneshwar Kumar</t>
+          <t xml:space="preserve"> Mohommad Shami</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -651,19 +651,19 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="L4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Kagiso Rabada</t>
+          <t xml:space="preserve"> Keshav Maharaj</t>
         </is>
       </c>
       <c r="O4" t="n">
@@ -677,19 +677,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Jasprit Bumrah</t>
+          <t xml:space="preserve"> Bhuvneshwar Kumar</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -701,10 +701,10 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="L5" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -713,7 +713,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Kagiso Rabada</t>
+          <t xml:space="preserve"> Dwaine Pretorius</t>
         </is>
       </c>
       <c r="O5" t="n">
@@ -727,10 +727,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C6" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -739,7 +739,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Kuldeep Yadav</t>
+          <t xml:space="preserve"> Mohommad Shami</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -751,19 +751,19 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Keshav Maharaj</t>
+          <t xml:space="preserve"> Dwaine Pretorius</t>
         </is>
       </c>
       <c r="O6" t="n">
@@ -777,10 +777,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="C7" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -789,7 +789,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Bhuvneshwar Kumar</t>
+          <t xml:space="preserve"> Hardik Pandya</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -801,19 +801,19 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="L7" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Kagiso Rabada</t>
+          <t xml:space="preserve"> Keshav Maharaj</t>
         </is>
       </c>
       <c r="O7" t="n">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -839,7 +839,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Hardik Pandya</t>
+          <t xml:space="preserve"> Kuldeep Yadav</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -854,16 +854,16 @@
         <v>14</v>
       </c>
       <c r="L8" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>LBW</t>
+          <t>NOT OUT</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tabraiz Shamsi</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="O8" t="n">
@@ -877,19 +877,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
         <v>6</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>LBW</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mohommad Shami</t>
+          <t xml:space="preserve"> Jasprit Bumrah</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -901,19 +901,19 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Caught</t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Anrich Nortje</t>
+          <t xml:space="preserve"> Keshav Maharaj</t>
         </is>
       </c>
       <c r="O9" t="n">
@@ -927,19 +927,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>* NOT OUT</t>
+          <t>Caught</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Jasprit Bumrah</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -951,10 +951,10 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L10" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -977,10 +977,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1001,14 +1001,14 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L11" t="n">
         <v>13</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>NOT OUT</t>
+          <t>* NOT OUT</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1030,16 +1030,16 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Bowled</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Mohommad Shami</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -1054,16 +1054,16 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Bowled</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Anrich Nortje</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="O12" t="n">
@@ -1114,32 +1114,32 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>307</v>
+        <v>186</v>
       </c>
       <c r="B16" t="n">
+        <v>10</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>12.2</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>74</v>
+      </c>
+      <c r="J16" t="n">
+        <v>189</v>
+      </c>
+      <c r="K16" t="n">
         <v>8</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>20.0</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>120</v>
-      </c>
-      <c r="J16" t="n">
-        <v>233</v>
-      </c>
-      <c r="K16" t="n">
-        <v>10</v>
-      </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>16.3</t>
+          <t>10.5</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>99</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20">
@@ -1197,201 +1197,201 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Kuldeep Yadav</t>
+          <t>Bhuvneshwar Kumar</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D21" t="n">
         <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>13.25</v>
+        <v>16</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Keshav Maharaj</t>
+          <t>Anrich Nortje</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>16.33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Jasprit Bumrah</t>
+          <t>Hardik Pandya</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Kagiso Rabada</t>
+          <t>Keshav Maharaj</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="M22" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N22" t="n">
-        <v>14</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Mohommad Shami</t>
+          <t>Kuldeep Yadav</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>15.5</v>
+        <v>16.67</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Dwaine Pretorius</t>
+          <t>Kagiso Rabada</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" t="n">
-        <v>14.33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Bhuvneshwar Kumar</t>
+          <t>Jasprit Bumrah</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="D24" t="n">
         <v>2</v>
       </c>
       <c r="E24" t="n">
-        <v>15</v>
+        <v>12.67</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Tabraiz Shamsi</t>
+          <t>Dwaine Pretorius</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="M24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N24" t="n">
-        <v>13.75</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Hardik Pandya</t>
+          <t>Mohommad Shami</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2.2</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25" t="n">
-        <v>15</v>
+        <v>15.45</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Anrich Nortje</t>
+          <t>Tabraiz Shamsi</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N25" t="n">
-        <v>13.33</v>
+        <v>17.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>